<commit_message>
SINED: 1) Aggiornamento dell'iter operativo dei casi di test 45 e 48 (timeout) nel file report-checklist.xlsx; 2)  riesecuzione dei casi di test 37 e 40 con conseguente ricompilazione dei file report-checklist.xlsx , data.json e rispedizione dei file PDF associati a questi due test.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SINEDXX/Sined S.r.l./MedWare/24.02.12/report-checklist.xlsx
+++ b/GATEWAY/A1#111SINEDXX/Sined S.r.l./MedWare/24.02.12/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my\fse001_ok_20240401.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my\fse001_ok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810DBB22-8F1E-4CB6-9CE2-33970FA0FD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5746F3-7E28-4221-8F29-77542E72B755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="973">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4669,15 +4669,6 @@
     <t>L'applicativo mostra a video l'errore evidenziato nella colonna N.  L'operatore contatta l'assistenza tecnica la quale, tramite i log dell'applicativo, identifica e  corregge l'errore comunicando, infine, la possibilità di ripetere la validazione</t>
   </si>
   <si>
-    <t>2024-04-03T13:47:52Z</t>
-  </si>
-  <si>
-    <t>5da9130d662b9e75</t>
-  </si>
-  <si>
-    <t>Campo token JWT non valido. - Il campo purpose_of_use non è corretto [403]</t>
-  </si>
-  <si>
     <t>Errore di timeout di connessione in fase di validazione FSE. Riprovare tra qualche minuto oppure contattare l'assistenza tecnica</t>
   </si>
   <si>
@@ -4822,9 +4813,6 @@
     <t>c236dc1ec690f67a</t>
   </si>
   <si>
-    <t>ef49fc30dad313f9</t>
-  </si>
-  <si>
     <t>2024-04-03T13:48:06Z</t>
   </si>
   <si>
@@ -5002,13 +4990,46 @@
     <t>2.16.840.1.113883.2.9.2.50.4.4.94e8ee451053fa110851408ed76dec6624a63f201402f62f1f92eaf8061114d3.e7770d63b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>L'applicativo mostra a video l'errore evidenziato nella colonna N. L'operatore, una volta effettuati n-tentativi come suggerito dalla segnalazione di errore, se il problema persiste, contatta l'assistenza tecnica la quale, tramite i log dell'applicativo, identifica e  corregge il problema comunicando, infine, la possibilità di ripetere la validazione</t>
-  </si>
-  <si>
     <t>Sined S.r.l.</t>
   </si>
   <si>
     <t>subject_application_vendor: Sined S.r.l.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A fronte di un errore di timeout, la procedura di integrazione, prima di comunicare all'operatore il messaggio di errore di colonna N, prova, per  un massimo di [X] volte ([X] = 2 per default), a rispedire in automatico il documento per essere 
+validato. Tutto questo, in maniera trasparente per l'operatore. Se, dopo [X] tentativi automatici, viene ancora restituito 
+timeout dal servizio di validazione, allora verrà segnalato l'errore di colonna N all'operatore, il quale, a questo punto, potrà : 
+- o riprovare subito a rispedire il documento per essere validato. Il numero di tentativi dipende dalla volontà dell'operatore;
+- o chiudere e, successivamente, quando lo desidera l'operatore stesso, riprendere in mano il documento e riprovare l'iter di validazione;
+- oppure, l'operatore potrà contattare l'assistenza tecnica di SINED la quale, tramite i log dell'applicativo, identificherà e,  se possibile correggerà il problema (se è in suo potere farlo) o contatterà chi lo potrà correggere, comunicando, infine, al ripristino del servizio, la possibilità di ripetere la validazione.
+A fronte di un errore di timeout, NON è prevista la gestione di una coda di documenti da validare con l'esecuzione automatica, 
+limitata ad un certo periodo, di tentativi automatici di validazione del documento .
+</t>
+  </si>
+  <si>
+    <t>A fronte di un errore di timeout, la procedura di integrazione, prima di comunicare all'operatore il messaggio di errore di colonna N, prova, per  un massimo di [X] volte ([X] = 2 per default), a rispedire in automatico il documento per essere 
+validato. Tutto questo, in maniera trasparente per l'operatore. Se, dopo [X] tentativi automatici, viene ancora restituito 
+timeout dal servizio di validazione, allora verrà segnalato l'errore di colonna N all'operatore, il quale, a questo punto, potrà : 
+- o riprovare subito a rispedire il documento per essere validato. Il numero di tentativi dipende dalla volontà dell'operatore;
+- o chiudere e, successivamente, quando lo desidera l'operatore stesso, riprendere in mano il documento e riprovare l'iter di validazione;
+- oppure, l'operatore potrà contattare l'assistenza tecnica di SINED la quale, tramite i log dell'applicativo, identificherà e,  se possibile correggerà il problema (se è in suo potere farlo) o contatterà chi lo potrà correggere, comunicando, infine, al ripristino del servizio, la possibilità di ripetere la validazione.
+A fronte di un errore di timeout, NON è prevista la gestione di una coda di documenti da validare con l'esecuzione automatica, 
+limitata ad un certo periodo, di tentativi automatici di validazione del documento .</t>
+  </si>
+  <si>
+    <t>2024-04-18T10:42:31Z</t>
+  </si>
+  <si>
+    <t>2024-04-18T10:43:30Z</t>
+  </si>
+  <si>
+    <t>cde993d684fa4385</t>
+  </si>
+  <si>
+    <t>45cd0d06c4ef2937</t>
+  </si>
+  <si>
+    <t>Campo token JWT non valido. - Il campo action_id non è corretto [403]</t>
   </si>
 </sst>
 </file>
@@ -5345,7 +5366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5460,6 +5481,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7945,10 +7969,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="N386" sqref="N386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7963,7 +7987,7 @@
     <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="36.44140625" customWidth="1"/>
-    <col min="16" max="16" width="40.109375" customWidth="1"/>
+    <col min="16" max="16" width="45.77734375" style="41" customWidth="1"/>
     <col min="17" max="17" width="33.109375" customWidth="1"/>
     <col min="18" max="18" width="36.44140625" customWidth="1"/>
     <col min="19" max="19" width="48.44140625" style="41" customWidth="1"/>
@@ -7982,21 +8006,21 @@
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="P1" s="38"/>
       <c r="Q1" s="13"/>
       <c r="R1" s="14"/>
       <c r="S1" s="38"/>
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46" t="s">
-        <v>969</v>
-      </c>
-      <c r="D2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47" t="s">
+        <v>964</v>
+      </c>
+      <c r="D2" s="46"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -8007,21 +8031,21 @@
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="P2" s="38"/>
       <c r="Q2" s="13"/>
       <c r="R2" s="14"/>
       <c r="S2" s="38"/>
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="54" t="s">
         <v>847</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="46"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -8032,19 +8056,19 @@
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
+      <c r="P3" s="38"/>
       <c r="Q3" s="13"/>
       <c r="R3" s="14"/>
       <c r="S3" s="38"/>
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="53" t="s">
-        <v>970</v>
-      </c>
-      <c r="D4" s="45"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="54" t="s">
+        <v>965</v>
+      </c>
+      <c r="D4" s="46"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -8056,19 +8080,19 @@
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
+      <c r="P4" s="38"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="14"/>
       <c r="S4" s="38"/>
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="54" t="s">
         <v>848</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="46"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -8079,15 +8103,15 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
+      <c r="P5" s="38"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="14"/>
       <c r="S5" s="38"/>
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="42"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -8099,7 +8123,7 @@
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
+      <c r="P6" s="38"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="14"/>
       <c r="S6" s="38"/>
@@ -8119,7 +8143,7 @@
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
+      <c r="P7" s="38"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="14"/>
       <c r="S7" s="38"/>
@@ -8136,7 +8160,7 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
+      <c r="P8" s="38"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="14"/>
       <c r="S8" s="38"/>
@@ -8188,7 +8212,7 @@
       <c r="O9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="39" t="s">
         <v>39</v>
       </c>
       <c r="Q9" s="18" t="s">
@@ -8444,7 +8468,7 @@
         <v>846</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -8454,7 +8478,7 @@
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
       <c r="S16" s="40" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="T16" s="28" t="s">
         <v>48</v>
@@ -8484,7 +8508,7 @@
         <v>846</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -8494,7 +8518,7 @@
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
       <c r="S17" s="40" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="T17" s="28" t="s">
         <v>48</v>
@@ -8524,7 +8548,7 @@
         <v>846</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -8534,7 +8558,7 @@
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
       <c r="S18" s="40" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="T18" s="28" t="s">
         <v>48</v>
@@ -9168,7 +9192,7 @@
       <c r="Q36" s="25"/>
       <c r="R36" s="26"/>
       <c r="S36" s="40" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="T36" s="28" t="s">
         <v>102</v>
@@ -9262,10 +9286,10 @@
         <v>45385</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="I39" s="24" t="s">
         <v>854</v>
@@ -9292,7 +9316,7 @@
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
       <c r="S39" s="27" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="T39" s="28" t="s">
         <v>102</v>
@@ -9451,13 +9475,13 @@
         <v>122</v>
       </c>
       <c r="F44" s="23">
-        <v>45385</v>
+        <v>45400</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>857</v>
+        <v>968</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>858</v>
+        <v>970</v>
       </c>
       <c r="I44" s="24" t="s">
         <v>854</v>
@@ -9473,7 +9497,7 @@
         <v>137</v>
       </c>
       <c r="N44" s="25" t="s">
-        <v>859</v>
+        <v>972</v>
       </c>
       <c r="O44" s="25" t="s">
         <v>137</v>
@@ -9484,7 +9508,7 @@
       <c r="Q44" s="25"/>
       <c r="R44" s="26"/>
       <c r="S44" s="40" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="T44" s="28" t="s">
         <v>102</v>
@@ -9575,13 +9599,13 @@
         <v>128</v>
       </c>
       <c r="F47" s="23">
-        <v>45385</v>
+        <v>45400</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>906</v>
+        <v>969</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>908</v>
+        <v>971</v>
       </c>
       <c r="I47" s="24" t="s">
         <v>854</v>
@@ -9597,7 +9621,7 @@
         <v>137</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>859</v>
+        <v>972</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>137</v>
@@ -9608,7 +9632,7 @@
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
       <c r="S47" s="27" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="T47" s="28" t="s">
         <v>102</v>
@@ -9752,7 +9776,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="37" customFormat="1" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" s="37" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="35">
         <v>45</v>
       </c>
@@ -9779,13 +9803,13 @@
       <c r="L52" s="25"/>
       <c r="M52" s="25"/>
       <c r="N52" s="25" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="O52" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="P52" s="25" t="s">
-        <v>968</v>
+      <c r="P52" s="42" t="s">
+        <v>966</v>
       </c>
       <c r="Q52" s="25"/>
       <c r="R52" s="26" t="s">
@@ -9868,7 +9892,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:20" s="37" customFormat="1" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" s="37" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="35">
         <v>48</v>
       </c>
@@ -9895,13 +9919,13 @@
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
       <c r="N55" s="25" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="O55" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="P55" s="25" t="s">
-        <v>968</v>
+      <c r="P55" s="42" t="s">
+        <v>967</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -10414,13 +10438,13 @@
         <v>45385</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>137</v>
@@ -10433,7 +10457,7 @@
         <v>137</v>
       </c>
       <c r="N70" s="25" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="O70" s="25" t="s">
         <v>137</v>
@@ -10444,7 +10468,7 @@
       <c r="Q70" s="25"/>
       <c r="R70" s="26"/>
       <c r="S70" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T70" s="28" t="s">
         <v>102</v>
@@ -10470,13 +10494,13 @@
         <v>45385</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="H71" s="24" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="J71" s="25" t="s">
         <v>137</v>
@@ -10489,7 +10513,7 @@
         <v>137</v>
       </c>
       <c r="N71" s="25" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="O71" s="25" t="s">
         <v>137</v>
@@ -10500,7 +10524,7 @@
       <c r="Q71" s="25"/>
       <c r="R71" s="26"/>
       <c r="S71" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T71" s="28" t="s">
         <v>102</v>
@@ -10526,13 +10550,13 @@
         <v>45385</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>137</v>
@@ -10545,7 +10569,7 @@
         <v>137</v>
       </c>
       <c r="N72" s="25" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="O72" s="25" t="s">
         <v>137</v>
@@ -10556,7 +10580,7 @@
       <c r="Q72" s="25"/>
       <c r="R72" s="26"/>
       <c r="S72" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T72" s="28" t="s">
         <v>102</v>
@@ -10582,13 +10606,13 @@
         <v>45385</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="H73" s="24" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="J73" s="25" t="s">
         <v>137</v>
@@ -10601,7 +10625,7 @@
         <v>137</v>
       </c>
       <c r="N73" s="25" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="O73" s="25" t="s">
         <v>137</v>
@@ -10612,7 +10636,7 @@
       <c r="Q73" s="25"/>
       <c r="R73" s="26"/>
       <c r="S73" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T73" s="28" t="s">
         <v>102</v>
@@ -10638,13 +10662,13 @@
         <v>45385</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="J74" s="25" t="s">
         <v>137</v>
@@ -10657,7 +10681,7 @@
         <v>137</v>
       </c>
       <c r="N74" s="25" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="O74" s="25" t="s">
         <v>137</v>
@@ -10668,7 +10692,7 @@
       <c r="Q74" s="25"/>
       <c r="R74" s="26"/>
       <c r="S74" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T74" s="28" t="s">
         <v>102</v>
@@ -10694,13 +10718,13 @@
         <v>45385</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="J75" s="25" t="s">
         <v>137</v>
@@ -10713,7 +10737,7 @@
         <v>137</v>
       </c>
       <c r="N75" s="25" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="O75" s="25" t="s">
         <v>137</v>
@@ -10724,7 +10748,7 @@
       <c r="Q75" s="25"/>
       <c r="R75" s="26"/>
       <c r="S75" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T75" s="28" t="s">
         <v>102</v>
@@ -10750,13 +10774,13 @@
         <v>45385</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="J76" s="25" t="s">
         <v>137</v>
@@ -10769,7 +10793,7 @@
         <v>137</v>
       </c>
       <c r="N76" s="25" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="O76" s="25" t="s">
         <v>137</v>
@@ -10780,7 +10804,7 @@
       <c r="Q76" s="25"/>
       <c r="R76" s="26"/>
       <c r="S76" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T76" s="28" t="s">
         <v>102</v>
@@ -10806,13 +10830,13 @@
         <v>45385</v>
       </c>
       <c r="G77" s="24" t="s">
+        <v>888</v>
+      </c>
+      <c r="H77" s="24" t="s">
+        <v>890</v>
+      </c>
+      <c r="I77" s="24" t="s">
         <v>891</v>
-      </c>
-      <c r="H77" s="24" t="s">
-        <v>893</v>
-      </c>
-      <c r="I77" s="24" t="s">
-        <v>894</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>137</v>
@@ -10825,7 +10849,7 @@
         <v>137</v>
       </c>
       <c r="N77" s="25" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="O77" s="25" t="s">
         <v>137</v>
@@ -10836,7 +10860,7 @@
       <c r="Q77" s="25"/>
       <c r="R77" s="26"/>
       <c r="S77" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T77" s="28" t="s">
         <v>102</v>
@@ -10866,7 +10890,7 @@
         <v>846</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="25"/>
@@ -10903,7 +10927,7 @@
         <v>846</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L79" s="25"/>
       <c r="M79" s="25"/>
@@ -10937,13 +10961,13 @@
         <v>45385</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="H80" s="24" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="I80" s="24" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="J80" s="25" t="s">
         <v>137</v>
@@ -10956,7 +10980,7 @@
         <v>137</v>
       </c>
       <c r="N80" s="25" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="O80" s="25" t="s">
         <v>137</v>
@@ -10967,7 +10991,7 @@
       <c r="Q80" s="25"/>
       <c r="R80" s="26"/>
       <c r="S80" s="40" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T80" s="28" t="s">
         <v>102</v>
@@ -10997,7 +11021,7 @@
         <v>846</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L81" s="25"/>
       <c r="M81" s="25"/>
@@ -13479,13 +13503,13 @@
         <v>45385</v>
       </c>
       <c r="G154" s="24" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="H154" s="24" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="I154" s="24" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="J154" s="25" t="s">
         <v>137</v>
@@ -13529,7 +13553,7 @@
         <v>846</v>
       </c>
       <c r="K155" s="25" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="L155" s="25"/>
       <c r="M155" s="25"/>
@@ -13539,7 +13563,7 @@
       <c r="Q155" s="25"/>
       <c r="R155" s="26"/>
       <c r="S155" s="27" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="T155" s="28" t="s">
         <v>48</v>
@@ -13569,7 +13593,7 @@
         <v>846</v>
       </c>
       <c r="K156" s="25" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -13579,7 +13603,7 @@
       <c r="Q156" s="25"/>
       <c r="R156" s="26"/>
       <c r="S156" s="27" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="T156" s="28" t="s">
         <v>48</v>
@@ -13609,7 +13633,7 @@
         <v>846</v>
       </c>
       <c r="K157" s="25" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -13619,7 +13643,7 @@
       <c r="Q157" s="25"/>
       <c r="R157" s="26"/>
       <c r="S157" s="27" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="T157" s="28" t="s">
         <v>48</v>
@@ -13645,13 +13669,13 @@
         <v>45385</v>
       </c>
       <c r="G158" s="24" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="H158" s="24" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="I158" s="24" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="J158" s="25" t="s">
         <v>137</v>
@@ -13664,7 +13688,7 @@
         <v>137</v>
       </c>
       <c r="N158" s="25" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="O158" s="25" t="s">
         <v>137</v>
@@ -13675,7 +13699,7 @@
       <c r="Q158" s="25"/>
       <c r="R158" s="26"/>
       <c r="S158" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T158" s="28" t="s">
         <v>102</v>
@@ -13701,13 +13725,13 @@
         <v>45385</v>
       </c>
       <c r="G159" s="24" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="H159" s="24" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="I159" s="37" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="J159" s="25" t="s">
         <v>137</v>
@@ -13720,7 +13744,7 @@
         <v>137</v>
       </c>
       <c r="N159" s="25" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="O159" s="25" t="s">
         <v>137</v>
@@ -13731,7 +13755,7 @@
       <c r="Q159" s="25"/>
       <c r="R159" s="26"/>
       <c r="S159" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T159" s="28" t="s">
         <v>102</v>
@@ -13757,13 +13781,13 @@
         <v>45385</v>
       </c>
       <c r="G160" s="24" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="H160" s="24" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="I160" s="24" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="J160" s="25" t="s">
         <v>137</v>
@@ -13776,7 +13800,7 @@
         <v>137</v>
       </c>
       <c r="N160" s="25" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="O160" s="25" t="s">
         <v>137</v>
@@ -13787,7 +13811,7 @@
       <c r="Q160" s="25"/>
       <c r="R160" s="26"/>
       <c r="S160" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T160" s="28" t="s">
         <v>102</v>
@@ -13813,13 +13837,13 @@
         <v>45385</v>
       </c>
       <c r="G161" s="24" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="H161" s="24" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="I161" s="24" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="J161" s="25" t="s">
         <v>137</v>
@@ -13832,7 +13856,7 @@
         <v>137</v>
       </c>
       <c r="N161" s="25" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="O161" s="25" t="s">
         <v>137</v>
@@ -13843,7 +13867,7 @@
       <c r="Q161" s="25"/>
       <c r="R161" s="26"/>
       <c r="S161" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T161" s="28" t="s">
         <v>102</v>
@@ -13869,13 +13893,13 @@
         <v>45385</v>
       </c>
       <c r="G162" s="24" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="H162" s="24" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="I162" s="24" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="J162" s="25" t="s">
         <v>137</v>
@@ -13888,7 +13912,7 @@
         <v>137</v>
       </c>
       <c r="N162" s="25" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="O162" s="25" t="s">
         <v>137</v>
@@ -13899,7 +13923,7 @@
       <c r="Q162" s="25"/>
       <c r="R162" s="26"/>
       <c r="S162" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T162" s="28" t="s">
         <v>102</v>
@@ -13925,13 +13949,13 @@
         <v>45385</v>
       </c>
       <c r="G163" s="24" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="H163" s="24" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="I163" s="24" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="J163" s="25" t="s">
         <v>137</v>
@@ -13944,7 +13968,7 @@
         <v>137</v>
       </c>
       <c r="N163" s="25" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="O163" s="25" t="s">
         <v>137</v>
@@ -13955,7 +13979,7 @@
       <c r="Q163" s="25"/>
       <c r="R163" s="26"/>
       <c r="S163" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T163" s="28" t="s">
         <v>102</v>
@@ -13985,7 +14009,7 @@
         <v>846</v>
       </c>
       <c r="K164" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L164" s="25"/>
       <c r="M164" s="25"/>
@@ -14019,13 +14043,13 @@
         <v>45385</v>
       </c>
       <c r="G165" s="24" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="H165" s="24" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="I165" s="24" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="J165" s="25" t="s">
         <v>137</v>
@@ -14038,7 +14062,7 @@
         <v>137</v>
       </c>
       <c r="N165" s="25" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="O165" s="25" t="s">
         <v>137</v>
@@ -14049,7 +14073,7 @@
       <c r="Q165" s="25"/>
       <c r="R165" s="26"/>
       <c r="S165" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T165" s="28" t="s">
         <v>102</v>
@@ -14075,13 +14099,13 @@
         <v>45385</v>
       </c>
       <c r="G166" s="24" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="H166" s="24" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="I166" s="24" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="J166" s="25" t="s">
         <v>137</v>
@@ -14094,7 +14118,7 @@
         <v>137</v>
       </c>
       <c r="N166" s="25" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="O166" s="25" t="s">
         <v>137</v>
@@ -14105,7 +14129,7 @@
       <c r="Q166" s="25"/>
       <c r="R166" s="26"/>
       <c r="S166" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T166" s="28" t="s">
         <v>102</v>
@@ -14131,13 +14155,13 @@
         <v>45385</v>
       </c>
       <c r="G167" s="24" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="H167" s="24" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="I167" s="24" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="J167" s="25" t="s">
         <v>137</v>
@@ -14150,7 +14174,7 @@
         <v>137</v>
       </c>
       <c r="N167" s="25" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="O167" s="25" t="s">
         <v>137</v>
@@ -14161,7 +14185,7 @@
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
       <c r="S167" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T167" s="28" t="s">
         <v>102</v>
@@ -14187,13 +14211,13 @@
         <v>45385</v>
       </c>
       <c r="G168" s="24" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="H168" s="24" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="I168" s="24" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="J168" s="25" t="s">
         <v>137</v>
@@ -14206,7 +14230,7 @@
         <v>137</v>
       </c>
       <c r="N168" s="25" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="O168" s="25" t="s">
         <v>137</v>
@@ -14217,7 +14241,7 @@
       <c r="Q168" s="25"/>
       <c r="R168" s="26"/>
       <c r="S168" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T168" s="28" t="s">
         <v>102</v>
@@ -14243,13 +14267,13 @@
         <v>45385</v>
       </c>
       <c r="G169" s="24" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="H169" s="24" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="I169" s="24" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="J169" s="25" t="s">
         <v>137</v>
@@ -14262,7 +14286,7 @@
         <v>137</v>
       </c>
       <c r="N169" s="25" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="O169" s="25" t="s">
         <v>137</v>
@@ -14273,7 +14297,7 @@
       <c r="Q169" s="25"/>
       <c r="R169" s="26"/>
       <c r="S169" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T169" s="28" t="s">
         <v>102</v>
@@ -14299,13 +14323,13 @@
         <v>45385</v>
       </c>
       <c r="G170" s="24" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="H170" s="24" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="I170" s="24" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="J170" s="25" t="s">
         <v>137</v>
@@ -14318,7 +14342,7 @@
         <v>137</v>
       </c>
       <c r="N170" s="25" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="O170" s="25" t="s">
         <v>137</v>
@@ -14329,7 +14353,7 @@
       <c r="Q170" s="25"/>
       <c r="R170" s="26"/>
       <c r="S170" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T170" s="28" t="s">
         <v>102</v>
@@ -14359,7 +14383,7 @@
         <v>846</v>
       </c>
       <c r="K171" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -14397,7 +14421,7 @@
         <v>846</v>
       </c>
       <c r="K172" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -14435,7 +14459,7 @@
         <v>846</v>
       </c>
       <c r="K173" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -14473,7 +14497,7 @@
         <v>846</v>
       </c>
       <c r="K174" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -14507,13 +14531,13 @@
         <v>45385</v>
       </c>
       <c r="G175" s="24" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="H175" s="24" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="I175" s="24" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="J175" s="25" t="s">
         <v>137</v>
@@ -14526,7 +14550,7 @@
         <v>137</v>
       </c>
       <c r="N175" s="25" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="O175" s="25" t="s">
         <v>137</v>
@@ -14537,7 +14561,7 @@
       <c r="Q175" s="25"/>
       <c r="R175" s="26"/>
       <c r="S175" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T175" s="28" t="s">
         <v>102</v>
@@ -14563,13 +14587,13 @@
         <v>45385</v>
       </c>
       <c r="G176" s="24" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="H176" s="24" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="I176" s="24" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="J176" s="25" t="s">
         <v>137</v>
@@ -14582,7 +14606,7 @@
         <v>137</v>
       </c>
       <c r="N176" s="25" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="O176" s="25" t="s">
         <v>137</v>
@@ -14593,7 +14617,7 @@
       <c r="Q176" s="25"/>
       <c r="R176" s="26"/>
       <c r="S176" s="27" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="T176" s="28" t="s">
         <v>102</v>
@@ -21385,13 +21409,13 @@
         <v>45385</v>
       </c>
       <c r="G376" s="24" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="H376" s="24" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="I376" s="24" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="J376" s="25" t="s">
         <v>137</v>
@@ -21565,13 +21589,13 @@
         <v>45385</v>
       </c>
       <c r="G381" s="24" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="H381" s="24" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="I381" s="24" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="J381" s="25" t="s">
         <v>137</v>
@@ -21668,7 +21692,7 @@
       <c r="M384" s="13"/>
       <c r="N384" s="13"/>
       <c r="O384" s="13"/>
-      <c r="P384" s="13"/>
+      <c r="P384" s="38"/>
       <c r="Q384" s="13"/>
       <c r="R384" s="14"/>
       <c r="S384" s="38"/>
@@ -21685,7 +21709,7 @@
       <c r="M385" s="13"/>
       <c r="N385" s="13"/>
       <c r="O385" s="13"/>
-      <c r="P385" s="13"/>
+      <c r="P385" s="38"/>
       <c r="Q385" s="13"/>
       <c r="R385" s="14"/>
       <c r="S385" s="38"/>
@@ -21702,7 +21726,7 @@
       <c r="M386" s="13"/>
       <c r="N386" s="13"/>
       <c r="O386" s="13"/>
-      <c r="P386" s="13"/>
+      <c r="P386" s="38"/>
       <c r="Q386" s="13"/>
       <c r="R386" s="14"/>
       <c r="S386" s="38"/>
@@ -21719,7 +21743,7 @@
       <c r="M387" s="13"/>
       <c r="N387" s="13"/>
       <c r="O387" s="13"/>
-      <c r="P387" s="13"/>
+      <c r="P387" s="38"/>
       <c r="Q387" s="13"/>
       <c r="R387" s="14"/>
       <c r="S387" s="38"/>
@@ -21736,7 +21760,7 @@
       <c r="M388" s="13"/>
       <c r="N388" s="13"/>
       <c r="O388" s="13"/>
-      <c r="P388" s="13"/>
+      <c r="P388" s="38"/>
       <c r="Q388" s="13"/>
       <c r="R388" s="14"/>
       <c r="S388" s="38"/>
@@ -21753,7 +21777,7 @@
       <c r="M389" s="13"/>
       <c r="N389" s="13"/>
       <c r="O389" s="13"/>
-      <c r="P389" s="13"/>
+      <c r="P389" s="38"/>
       <c r="Q389" s="13"/>
       <c r="R389" s="14"/>
       <c r="S389" s="38"/>
@@ -21770,7 +21794,7 @@
       <c r="M390" s="13"/>
       <c r="N390" s="13"/>
       <c r="O390" s="13"/>
-      <c r="P390" s="13"/>
+      <c r="P390" s="38"/>
       <c r="Q390" s="13"/>
       <c r="R390" s="14"/>
       <c r="S390" s="38"/>
@@ -21787,7 +21811,7 @@
       <c r="M391" s="13"/>
       <c r="N391" s="13"/>
       <c r="O391" s="13"/>
-      <c r="P391" s="13"/>
+      <c r="P391" s="38"/>
       <c r="Q391" s="13"/>
       <c r="R391" s="14"/>
       <c r="S391" s="38"/>
@@ -21804,7 +21828,7 @@
       <c r="M392" s="13"/>
       <c r="N392" s="13"/>
       <c r="O392" s="13"/>
-      <c r="P392" s="13"/>
+      <c r="P392" s="38"/>
       <c r="Q392" s="13"/>
       <c r="R392" s="14"/>
       <c r="S392" s="38"/>
@@ -21821,7 +21845,7 @@
       <c r="M393" s="13"/>
       <c r="N393" s="13"/>
       <c r="O393" s="13"/>
-      <c r="P393" s="13"/>
+      <c r="P393" s="38"/>
       <c r="Q393" s="13"/>
       <c r="R393" s="14"/>
       <c r="S393" s="38"/>
@@ -21838,7 +21862,7 @@
       <c r="M394" s="13"/>
       <c r="N394" s="13"/>
       <c r="O394" s="13"/>
-      <c r="P394" s="13"/>
+      <c r="P394" s="38"/>
       <c r="Q394" s="13"/>
       <c r="R394" s="14"/>
       <c r="S394" s="38"/>
@@ -21855,7 +21879,7 @@
       <c r="M395" s="13"/>
       <c r="N395" s="13"/>
       <c r="O395" s="13"/>
-      <c r="P395" s="13"/>
+      <c r="P395" s="38"/>
       <c r="Q395" s="13"/>
       <c r="R395" s="14"/>
       <c r="S395" s="38"/>
@@ -21872,7 +21896,7 @@
       <c r="M396" s="13"/>
       <c r="N396" s="13"/>
       <c r="O396" s="13"/>
-      <c r="P396" s="13"/>
+      <c r="P396" s="38"/>
       <c r="Q396" s="13"/>
       <c r="R396" s="14"/>
       <c r="S396" s="38"/>
@@ -21889,7 +21913,7 @@
       <c r="M397" s="13"/>
       <c r="N397" s="13"/>
       <c r="O397" s="13"/>
-      <c r="P397" s="13"/>
+      <c r="P397" s="38"/>
       <c r="Q397" s="13"/>
       <c r="R397" s="14"/>
       <c r="S397" s="38"/>
@@ -21906,7 +21930,7 @@
       <c r="M398" s="13"/>
       <c r="N398" s="13"/>
       <c r="O398" s="13"/>
-      <c r="P398" s="13"/>
+      <c r="P398" s="38"/>
       <c r="Q398" s="13"/>
       <c r="R398" s="14"/>
       <c r="S398" s="38"/>
@@ -21923,7 +21947,7 @@
       <c r="M399" s="13"/>
       <c r="N399" s="13"/>
       <c r="O399" s="13"/>
-      <c r="P399" s="13"/>
+      <c r="P399" s="38"/>
       <c r="Q399" s="13"/>
       <c r="R399" s="14"/>
       <c r="S399" s="38"/>
@@ -21940,7 +21964,7 @@
       <c r="M400" s="13"/>
       <c r="N400" s="13"/>
       <c r="O400" s="13"/>
-      <c r="P400" s="13"/>
+      <c r="P400" s="38"/>
       <c r="Q400" s="13"/>
       <c r="R400" s="14"/>
       <c r="S400" s="38"/>
@@ -21957,7 +21981,7 @@
       <c r="M401" s="13"/>
       <c r="N401" s="13"/>
       <c r="O401" s="13"/>
-      <c r="P401" s="13"/>
+      <c r="P401" s="38"/>
       <c r="Q401" s="13"/>
       <c r="R401" s="14"/>
       <c r="S401" s="38"/>
@@ -21974,7 +21998,7 @@
       <c r="M402" s="13"/>
       <c r="N402" s="13"/>
       <c r="O402" s="13"/>
-      <c r="P402" s="13"/>
+      <c r="P402" s="38"/>
       <c r="Q402" s="13"/>
       <c r="R402" s="14"/>
       <c r="S402" s="38"/>
@@ -21991,7 +22015,7 @@
       <c r="M403" s="13"/>
       <c r="N403" s="13"/>
       <c r="O403" s="13"/>
-      <c r="P403" s="13"/>
+      <c r="P403" s="38"/>
       <c r="Q403" s="13"/>
       <c r="R403" s="14"/>
       <c r="S403" s="38"/>
@@ -22008,7 +22032,7 @@
       <c r="M404" s="13"/>
       <c r="N404" s="13"/>
       <c r="O404" s="13"/>
-      <c r="P404" s="13"/>
+      <c r="P404" s="38"/>
       <c r="Q404" s="13"/>
       <c r="R404" s="14"/>
       <c r="S404" s="38"/>
@@ -22025,7 +22049,7 @@
       <c r="M405" s="13"/>
       <c r="N405" s="13"/>
       <c r="O405" s="13"/>
-      <c r="P405" s="13"/>
+      <c r="P405" s="38"/>
       <c r="Q405" s="13"/>
       <c r="R405" s="14"/>
       <c r="S405" s="38"/>
@@ -22042,7 +22066,7 @@
       <c r="M406" s="13"/>
       <c r="N406" s="13"/>
       <c r="O406" s="13"/>
-      <c r="P406" s="13"/>
+      <c r="P406" s="38"/>
       <c r="Q406" s="13"/>
       <c r="R406" s="14"/>
       <c r="S406" s="38"/>
@@ -22059,7 +22083,7 @@
       <c r="M407" s="13"/>
       <c r="N407" s="13"/>
       <c r="O407" s="13"/>
-      <c r="P407" s="13"/>
+      <c r="P407" s="38"/>
       <c r="Q407" s="13"/>
       <c r="R407" s="14"/>
       <c r="S407" s="38"/>
@@ -22076,7 +22100,7 @@
       <c r="M408" s="13"/>
       <c r="N408" s="13"/>
       <c r="O408" s="13"/>
-      <c r="P408" s="13"/>
+      <c r="P408" s="38"/>
       <c r="Q408" s="13"/>
       <c r="R408" s="14"/>
       <c r="S408" s="38"/>
@@ -22093,7 +22117,7 @@
       <c r="M409" s="13"/>
       <c r="N409" s="13"/>
       <c r="O409" s="13"/>
-      <c r="P409" s="13"/>
+      <c r="P409" s="38"/>
       <c r="Q409" s="13"/>
       <c r="R409" s="14"/>
       <c r="S409" s="38"/>
@@ -22110,7 +22134,7 @@
       <c r="M410" s="13"/>
       <c r="N410" s="13"/>
       <c r="O410" s="13"/>
-      <c r="P410" s="13"/>
+      <c r="P410" s="38"/>
       <c r="Q410" s="13"/>
       <c r="R410" s="14"/>
       <c r="S410" s="38"/>
@@ -22127,7 +22151,7 @@
       <c r="M411" s="13"/>
       <c r="N411" s="13"/>
       <c r="O411" s="13"/>
-      <c r="P411" s="13"/>
+      <c r="P411" s="38"/>
       <c r="Q411" s="13"/>
       <c r="R411" s="14"/>
       <c r="S411" s="38"/>
@@ -22144,7 +22168,7 @@
       <c r="M412" s="13"/>
       <c r="N412" s="13"/>
       <c r="O412" s="13"/>
-      <c r="P412" s="13"/>
+      <c r="P412" s="38"/>
       <c r="Q412" s="13"/>
       <c r="R412" s="14"/>
       <c r="S412" s="38"/>
@@ -22161,7 +22185,7 @@
       <c r="M413" s="13"/>
       <c r="N413" s="13"/>
       <c r="O413" s="13"/>
-      <c r="P413" s="13"/>
+      <c r="P413" s="38"/>
       <c r="Q413" s="13"/>
       <c r="R413" s="14"/>
       <c r="S413" s="38"/>
@@ -22178,7 +22202,7 @@
       <c r="M414" s="13"/>
       <c r="N414" s="13"/>
       <c r="O414" s="13"/>
-      <c r="P414" s="13"/>
+      <c r="P414" s="38"/>
       <c r="Q414" s="13"/>
       <c r="R414" s="14"/>
       <c r="S414" s="38"/>
@@ -22195,7 +22219,7 @@
       <c r="M415" s="13"/>
       <c r="N415" s="13"/>
       <c r="O415" s="13"/>
-      <c r="P415" s="13"/>
+      <c r="P415" s="38"/>
       <c r="Q415" s="13"/>
       <c r="R415" s="14"/>
       <c r="S415" s="38"/>
@@ -22212,7 +22236,7 @@
       <c r="M416" s="13"/>
       <c r="N416" s="13"/>
       <c r="O416" s="13"/>
-      <c r="P416" s="13"/>
+      <c r="P416" s="38"/>
       <c r="Q416" s="13"/>
       <c r="R416" s="14"/>
       <c r="S416" s="38"/>
@@ -22229,7 +22253,7 @@
       <c r="M417" s="13"/>
       <c r="N417" s="13"/>
       <c r="O417" s="13"/>
-      <c r="P417" s="13"/>
+      <c r="P417" s="38"/>
       <c r="Q417" s="13"/>
       <c r="R417" s="14"/>
       <c r="S417" s="38"/>
@@ -22246,7 +22270,7 @@
       <c r="M418" s="13"/>
       <c r="N418" s="13"/>
       <c r="O418" s="13"/>
-      <c r="P418" s="13"/>
+      <c r="P418" s="38"/>
       <c r="Q418" s="13"/>
       <c r="R418" s="14"/>
       <c r="S418" s="38"/>
@@ -22263,7 +22287,7 @@
       <c r="M419" s="13"/>
       <c r="N419" s="13"/>
       <c r="O419" s="13"/>
-      <c r="P419" s="13"/>
+      <c r="P419" s="38"/>
       <c r="Q419" s="13"/>
       <c r="R419" s="14"/>
       <c r="S419" s="38"/>
@@ -22280,7 +22304,7 @@
       <c r="M420" s="13"/>
       <c r="N420" s="13"/>
       <c r="O420" s="13"/>
-      <c r="P420" s="13"/>
+      <c r="P420" s="38"/>
       <c r="Q420" s="13"/>
       <c r="R420" s="14"/>
       <c r="S420" s="38"/>
@@ -22297,7 +22321,7 @@
       <c r="M421" s="13"/>
       <c r="N421" s="13"/>
       <c r="O421" s="13"/>
-      <c r="P421" s="13"/>
+      <c r="P421" s="38"/>
       <c r="Q421" s="13"/>
       <c r="R421" s="14"/>
       <c r="S421" s="38"/>
@@ -22314,7 +22338,7 @@
       <c r="M422" s="13"/>
       <c r="N422" s="13"/>
       <c r="O422" s="13"/>
-      <c r="P422" s="13"/>
+      <c r="P422" s="38"/>
       <c r="Q422" s="13"/>
       <c r="R422" s="14"/>
       <c r="S422" s="38"/>
@@ -22331,7 +22355,7 @@
       <c r="M423" s="13"/>
       <c r="N423" s="13"/>
       <c r="O423" s="13"/>
-      <c r="P423" s="13"/>
+      <c r="P423" s="38"/>
       <c r="Q423" s="13"/>
       <c r="R423" s="14"/>
       <c r="S423" s="38"/>
@@ -22348,7 +22372,7 @@
       <c r="M424" s="13"/>
       <c r="N424" s="13"/>
       <c r="O424" s="13"/>
-      <c r="P424" s="13"/>
+      <c r="P424" s="38"/>
       <c r="Q424" s="13"/>
       <c r="R424" s="14"/>
       <c r="S424" s="38"/>
@@ -22365,7 +22389,7 @@
       <c r="M425" s="13"/>
       <c r="N425" s="13"/>
       <c r="O425" s="13"/>
-      <c r="P425" s="13"/>
+      <c r="P425" s="38"/>
       <c r="Q425" s="13"/>
       <c r="R425" s="14"/>
       <c r="S425" s="38"/>
@@ -22382,7 +22406,7 @@
       <c r="M426" s="13"/>
       <c r="N426" s="13"/>
       <c r="O426" s="13"/>
-      <c r="P426" s="13"/>
+      <c r="P426" s="38"/>
       <c r="Q426" s="13"/>
       <c r="R426" s="14"/>
       <c r="S426" s="38"/>
@@ -22399,7 +22423,7 @@
       <c r="M427" s="13"/>
       <c r="N427" s="13"/>
       <c r="O427" s="13"/>
-      <c r="P427" s="13"/>
+      <c r="P427" s="38"/>
       <c r="Q427" s="13"/>
       <c r="R427" s="14"/>
       <c r="S427" s="38"/>
@@ -22416,7 +22440,7 @@
       <c r="M428" s="13"/>
       <c r="N428" s="13"/>
       <c r="O428" s="13"/>
-      <c r="P428" s="13"/>
+      <c r="P428" s="38"/>
       <c r="Q428" s="13"/>
       <c r="R428" s="14"/>
       <c r="S428" s="38"/>
@@ -22433,7 +22457,7 @@
       <c r="M429" s="13"/>
       <c r="N429" s="13"/>
       <c r="O429" s="13"/>
-      <c r="P429" s="13"/>
+      <c r="P429" s="38"/>
       <c r="Q429" s="13"/>
       <c r="R429" s="14"/>
       <c r="S429" s="38"/>
@@ -22450,7 +22474,7 @@
       <c r="M430" s="13"/>
       <c r="N430" s="13"/>
       <c r="O430" s="13"/>
-      <c r="P430" s="13"/>
+      <c r="P430" s="38"/>
       <c r="Q430" s="13"/>
       <c r="R430" s="14"/>
       <c r="S430" s="38"/>
@@ -22467,7 +22491,7 @@
       <c r="M431" s="13"/>
       <c r="N431" s="13"/>
       <c r="O431" s="13"/>
-      <c r="P431" s="13"/>
+      <c r="P431" s="38"/>
       <c r="Q431" s="13"/>
       <c r="R431" s="14"/>
       <c r="S431" s="38"/>
@@ -22484,7 +22508,7 @@
       <c r="M432" s="13"/>
       <c r="N432" s="13"/>
       <c r="O432" s="13"/>
-      <c r="P432" s="13"/>
+      <c r="P432" s="38"/>
       <c r="Q432" s="13"/>
       <c r="R432" s="14"/>
       <c r="S432" s="38"/>
@@ -22501,7 +22525,7 @@
       <c r="M433" s="13"/>
       <c r="N433" s="13"/>
       <c r="O433" s="13"/>
-      <c r="P433" s="13"/>
+      <c r="P433" s="38"/>
       <c r="Q433" s="13"/>
       <c r="R433" s="14"/>
       <c r="S433" s="38"/>
@@ -22518,7 +22542,7 @@
       <c r="M434" s="13"/>
       <c r="N434" s="13"/>
       <c r="O434" s="13"/>
-      <c r="P434" s="13"/>
+      <c r="P434" s="38"/>
       <c r="Q434" s="13"/>
       <c r="R434" s="14"/>
       <c r="S434" s="38"/>
@@ -22535,7 +22559,7 @@
       <c r="M435" s="13"/>
       <c r="N435" s="13"/>
       <c r="O435" s="13"/>
-      <c r="P435" s="13"/>
+      <c r="P435" s="38"/>
       <c r="Q435" s="13"/>
       <c r="R435" s="14"/>
       <c r="S435" s="38"/>
@@ -22552,7 +22576,7 @@
       <c r="M436" s="13"/>
       <c r="N436" s="13"/>
       <c r="O436" s="13"/>
-      <c r="P436" s="13"/>
+      <c r="P436" s="38"/>
       <c r="Q436" s="13"/>
       <c r="R436" s="14"/>
       <c r="S436" s="38"/>
@@ -22569,7 +22593,7 @@
       <c r="M437" s="13"/>
       <c r="N437" s="13"/>
       <c r="O437" s="13"/>
-      <c r="P437" s="13"/>
+      <c r="P437" s="38"/>
       <c r="Q437" s="13"/>
       <c r="R437" s="14"/>
       <c r="S437" s="38"/>
@@ -22586,7 +22610,7 @@
       <c r="M438" s="13"/>
       <c r="N438" s="13"/>
       <c r="O438" s="13"/>
-      <c r="P438" s="13"/>
+      <c r="P438" s="38"/>
       <c r="Q438" s="13"/>
       <c r="R438" s="14"/>
       <c r="S438" s="38"/>
@@ -22603,7 +22627,7 @@
       <c r="M439" s="13"/>
       <c r="N439" s="13"/>
       <c r="O439" s="13"/>
-      <c r="P439" s="13"/>
+      <c r="P439" s="38"/>
       <c r="Q439" s="13"/>
       <c r="R439" s="14"/>
       <c r="S439" s="38"/>
@@ -22620,7 +22644,7 @@
       <c r="M440" s="13"/>
       <c r="N440" s="13"/>
       <c r="O440" s="13"/>
-      <c r="P440" s="13"/>
+      <c r="P440" s="38"/>
       <c r="Q440" s="13"/>
       <c r="R440" s="14"/>
       <c r="S440" s="38"/>
@@ -22637,7 +22661,7 @@
       <c r="M441" s="13"/>
       <c r="N441" s="13"/>
       <c r="O441" s="13"/>
-      <c r="P441" s="13"/>
+      <c r="P441" s="38"/>
       <c r="Q441" s="13"/>
       <c r="R441" s="14"/>
       <c r="S441" s="38"/>
@@ -22654,7 +22678,7 @@
       <c r="M442" s="13"/>
       <c r="N442" s="13"/>
       <c r="O442" s="13"/>
-      <c r="P442" s="13"/>
+      <c r="P442" s="38"/>
       <c r="Q442" s="13"/>
       <c r="R442" s="14"/>
       <c r="S442" s="38"/>
@@ -22671,7 +22695,7 @@
       <c r="M443" s="13"/>
       <c r="N443" s="13"/>
       <c r="O443" s="13"/>
-      <c r="P443" s="13"/>
+      <c r="P443" s="38"/>
       <c r="Q443" s="13"/>
       <c r="R443" s="14"/>
       <c r="S443" s="38"/>
@@ -22688,7 +22712,7 @@
       <c r="M444" s="13"/>
       <c r="N444" s="13"/>
       <c r="O444" s="13"/>
-      <c r="P444" s="13"/>
+      <c r="P444" s="38"/>
       <c r="Q444" s="13"/>
       <c r="R444" s="14"/>
       <c r="S444" s="38"/>
@@ -22705,7 +22729,7 @@
       <c r="M445" s="13"/>
       <c r="N445" s="13"/>
       <c r="O445" s="13"/>
-      <c r="P445" s="13"/>
+      <c r="P445" s="38"/>
       <c r="Q445" s="13"/>
       <c r="R445" s="14"/>
       <c r="S445" s="38"/>
@@ -22722,7 +22746,7 @@
       <c r="M446" s="13"/>
       <c r="N446" s="13"/>
       <c r="O446" s="13"/>
-      <c r="P446" s="13"/>
+      <c r="P446" s="38"/>
       <c r="Q446" s="13"/>
       <c r="R446" s="14"/>
       <c r="S446" s="38"/>
@@ -22739,7 +22763,7 @@
       <c r="M447" s="13"/>
       <c r="N447" s="13"/>
       <c r="O447" s="13"/>
-      <c r="P447" s="13"/>
+      <c r="P447" s="38"/>
       <c r="Q447" s="13"/>
       <c r="R447" s="14"/>
       <c r="S447" s="38"/>
@@ -22756,7 +22780,7 @@
       <c r="M448" s="13"/>
       <c r="N448" s="13"/>
       <c r="O448" s="13"/>
-      <c r="P448" s="13"/>
+      <c r="P448" s="38"/>
       <c r="Q448" s="13"/>
       <c r="R448" s="14"/>
       <c r="S448" s="38"/>
@@ -22773,7 +22797,7 @@
       <c r="M449" s="13"/>
       <c r="N449" s="13"/>
       <c r="O449" s="13"/>
-      <c r="P449" s="13"/>
+      <c r="P449" s="38"/>
       <c r="Q449" s="13"/>
       <c r="R449" s="14"/>
       <c r="S449" s="38"/>
@@ -22790,7 +22814,7 @@
       <c r="M450" s="13"/>
       <c r="N450" s="13"/>
       <c r="O450" s="13"/>
-      <c r="P450" s="13"/>
+      <c r="P450" s="38"/>
       <c r="Q450" s="13"/>
       <c r="R450" s="14"/>
       <c r="S450" s="38"/>
@@ -22807,7 +22831,7 @@
       <c r="M451" s="13"/>
       <c r="N451" s="13"/>
       <c r="O451" s="13"/>
-      <c r="P451" s="13"/>
+      <c r="P451" s="38"/>
       <c r="Q451" s="13"/>
       <c r="R451" s="14"/>
       <c r="S451" s="38"/>
@@ -22824,7 +22848,7 @@
       <c r="M452" s="13"/>
       <c r="N452" s="13"/>
       <c r="O452" s="13"/>
-      <c r="P452" s="13"/>
+      <c r="P452" s="38"/>
       <c r="Q452" s="13"/>
       <c r="R452" s="14"/>
       <c r="S452" s="38"/>
@@ -22841,7 +22865,7 @@
       <c r="M453" s="13"/>
       <c r="N453" s="13"/>
       <c r="O453" s="13"/>
-      <c r="P453" s="13"/>
+      <c r="P453" s="38"/>
       <c r="Q453" s="13"/>
       <c r="R453" s="14"/>
       <c r="S453" s="38"/>
@@ -22858,7 +22882,7 @@
       <c r="M454" s="13"/>
       <c r="N454" s="13"/>
       <c r="O454" s="13"/>
-      <c r="P454" s="13"/>
+      <c r="P454" s="38"/>
       <c r="Q454" s="13"/>
       <c r="R454" s="14"/>
       <c r="S454" s="38"/>
@@ -22875,7 +22899,7 @@
       <c r="M455" s="13"/>
       <c r="N455" s="13"/>
       <c r="O455" s="13"/>
-      <c r="P455" s="13"/>
+      <c r="P455" s="38"/>
       <c r="Q455" s="13"/>
       <c r="R455" s="14"/>
       <c r="S455" s="38"/>
@@ -22892,7 +22916,7 @@
       <c r="M456" s="13"/>
       <c r="N456" s="13"/>
       <c r="O456" s="13"/>
-      <c r="P456" s="13"/>
+      <c r="P456" s="38"/>
       <c r="Q456" s="13"/>
       <c r="R456" s="14"/>
       <c r="S456" s="38"/>
@@ -22909,7 +22933,7 @@
       <c r="M457" s="13"/>
       <c r="N457" s="13"/>
       <c r="O457" s="13"/>
-      <c r="P457" s="13"/>
+      <c r="P457" s="38"/>
       <c r="Q457" s="13"/>
       <c r="R457" s="14"/>
       <c r="S457" s="38"/>
@@ -22926,7 +22950,7 @@
       <c r="M458" s="13"/>
       <c r="N458" s="13"/>
       <c r="O458" s="13"/>
-      <c r="P458" s="13"/>
+      <c r="P458" s="38"/>
       <c r="Q458" s="13"/>
       <c r="R458" s="14"/>
       <c r="S458" s="38"/>
@@ -22943,7 +22967,7 @@
       <c r="M459" s="13"/>
       <c r="N459" s="13"/>
       <c r="O459" s="13"/>
-      <c r="P459" s="13"/>
+      <c r="P459" s="38"/>
       <c r="Q459" s="13"/>
       <c r="R459" s="14"/>
       <c r="S459" s="38"/>
@@ -22960,7 +22984,7 @@
       <c r="M460" s="13"/>
       <c r="N460" s="13"/>
       <c r="O460" s="13"/>
-      <c r="P460" s="13"/>
+      <c r="P460" s="38"/>
       <c r="Q460" s="13"/>
       <c r="R460" s="14"/>
       <c r="S460" s="38"/>
@@ -22977,7 +23001,7 @@
       <c r="M461" s="13"/>
       <c r="N461" s="13"/>
       <c r="O461" s="13"/>
-      <c r="P461" s="13"/>
+      <c r="P461" s="38"/>
       <c r="Q461" s="13"/>
       <c r="R461" s="14"/>
       <c r="S461" s="38"/>
@@ -22994,7 +23018,7 @@
       <c r="M462" s="13"/>
       <c r="N462" s="13"/>
       <c r="O462" s="13"/>
-      <c r="P462" s="13"/>
+      <c r="P462" s="38"/>
       <c r="Q462" s="13"/>
       <c r="R462" s="14"/>
       <c r="S462" s="38"/>
@@ -23011,7 +23035,7 @@
       <c r="M463" s="13"/>
       <c r="N463" s="13"/>
       <c r="O463" s="13"/>
-      <c r="P463" s="13"/>
+      <c r="P463" s="38"/>
       <c r="Q463" s="13"/>
       <c r="R463" s="14"/>
       <c r="S463" s="38"/>
@@ -23028,7 +23052,7 @@
       <c r="M464" s="13"/>
       <c r="N464" s="13"/>
       <c r="O464" s="13"/>
-      <c r="P464" s="13"/>
+      <c r="P464" s="38"/>
       <c r="Q464" s="13"/>
       <c r="R464" s="14"/>
       <c r="S464" s="38"/>
@@ -23045,7 +23069,7 @@
       <c r="M465" s="13"/>
       <c r="N465" s="13"/>
       <c r="O465" s="13"/>
-      <c r="P465" s="13"/>
+      <c r="P465" s="38"/>
       <c r="Q465" s="13"/>
       <c r="R465" s="14"/>
       <c r="S465" s="38"/>
@@ -23062,7 +23086,7 @@
       <c r="M466" s="13"/>
       <c r="N466" s="13"/>
       <c r="O466" s="13"/>
-      <c r="P466" s="13"/>
+      <c r="P466" s="38"/>
       <c r="Q466" s="13"/>
       <c r="R466" s="14"/>
       <c r="S466" s="38"/>
@@ -23079,7 +23103,7 @@
       <c r="M467" s="13"/>
       <c r="N467" s="13"/>
       <c r="O467" s="13"/>
-      <c r="P467" s="13"/>
+      <c r="P467" s="38"/>
       <c r="Q467" s="13"/>
       <c r="R467" s="14"/>
       <c r="S467" s="38"/>
@@ -23096,7 +23120,7 @@
       <c r="M468" s="13"/>
       <c r="N468" s="13"/>
       <c r="O468" s="13"/>
-      <c r="P468" s="13"/>
+      <c r="P468" s="38"/>
       <c r="Q468" s="13"/>
       <c r="R468" s="14"/>
       <c r="S468" s="38"/>
@@ -23113,7 +23137,7 @@
       <c r="M469" s="13"/>
       <c r="N469" s="13"/>
       <c r="O469" s="13"/>
-      <c r="P469" s="13"/>
+      <c r="P469" s="38"/>
       <c r="Q469" s="13"/>
       <c r="R469" s="14"/>
       <c r="S469" s="38"/>
@@ -23130,7 +23154,7 @@
       <c r="M470" s="13"/>
       <c r="N470" s="13"/>
       <c r="O470" s="13"/>
-      <c r="P470" s="13"/>
+      <c r="P470" s="38"/>
       <c r="Q470" s="13"/>
       <c r="R470" s="14"/>
       <c r="S470" s="38"/>
@@ -23147,7 +23171,7 @@
       <c r="M471" s="13"/>
       <c r="N471" s="13"/>
       <c r="O471" s="13"/>
-      <c r="P471" s="13"/>
+      <c r="P471" s="38"/>
       <c r="Q471" s="13"/>
       <c r="R471" s="14"/>
       <c r="S471" s="38"/>
@@ -23164,7 +23188,7 @@
       <c r="M472" s="13"/>
       <c r="N472" s="13"/>
       <c r="O472" s="13"/>
-      <c r="P472" s="13"/>
+      <c r="P472" s="38"/>
       <c r="Q472" s="13"/>
       <c r="R472" s="14"/>
       <c r="S472" s="38"/>
@@ -23181,7 +23205,7 @@
       <c r="M473" s="13"/>
       <c r="N473" s="13"/>
       <c r="O473" s="13"/>
-      <c r="P473" s="13"/>
+      <c r="P473" s="38"/>
       <c r="Q473" s="13"/>
       <c r="R473" s="14"/>
       <c r="S473" s="38"/>
@@ -23198,7 +23222,7 @@
       <c r="M474" s="13"/>
       <c r="N474" s="13"/>
       <c r="O474" s="13"/>
-      <c r="P474" s="13"/>
+      <c r="P474" s="38"/>
       <c r="Q474" s="13"/>
       <c r="R474" s="14"/>
       <c r="S474" s="38"/>
@@ -23215,7 +23239,7 @@
       <c r="M475" s="13"/>
       <c r="N475" s="13"/>
       <c r="O475" s="13"/>
-      <c r="P475" s="13"/>
+      <c r="P475" s="38"/>
       <c r="Q475" s="13"/>
       <c r="R475" s="14"/>
       <c r="S475" s="38"/>
@@ -23232,7 +23256,7 @@
       <c r="M476" s="13"/>
       <c r="N476" s="13"/>
       <c r="O476" s="13"/>
-      <c r="P476" s="13"/>
+      <c r="P476" s="38"/>
       <c r="Q476" s="13"/>
       <c r="R476" s="14"/>
       <c r="S476" s="38"/>
@@ -23249,7 +23273,7 @@
       <c r="M477" s="13"/>
       <c r="N477" s="13"/>
       <c r="O477" s="13"/>
-      <c r="P477" s="13"/>
+      <c r="P477" s="38"/>
       <c r="Q477" s="13"/>
       <c r="R477" s="14"/>
       <c r="S477" s="38"/>
@@ -23266,7 +23290,7 @@
       <c r="M478" s="13"/>
       <c r="N478" s="13"/>
       <c r="O478" s="13"/>
-      <c r="P478" s="13"/>
+      <c r="P478" s="38"/>
       <c r="Q478" s="13"/>
       <c r="R478" s="14"/>
       <c r="S478" s="38"/>
@@ -23283,7 +23307,7 @@
       <c r="M479" s="13"/>
       <c r="N479" s="13"/>
       <c r="O479" s="13"/>
-      <c r="P479" s="13"/>
+      <c r="P479" s="38"/>
       <c r="Q479" s="13"/>
       <c r="R479" s="14"/>
       <c r="S479" s="38"/>
@@ -23300,7 +23324,7 @@
       <c r="M480" s="13"/>
       <c r="N480" s="13"/>
       <c r="O480" s="13"/>
-      <c r="P480" s="13"/>
+      <c r="P480" s="38"/>
       <c r="Q480" s="13"/>
       <c r="R480" s="14"/>
       <c r="S480" s="38"/>
@@ -23317,7 +23341,7 @@
       <c r="M481" s="13"/>
       <c r="N481" s="13"/>
       <c r="O481" s="13"/>
-      <c r="P481" s="13"/>
+      <c r="P481" s="38"/>
       <c r="Q481" s="13"/>
       <c r="R481" s="14"/>
       <c r="S481" s="38"/>
@@ -23334,7 +23358,7 @@
       <c r="M482" s="13"/>
       <c r="N482" s="13"/>
       <c r="O482" s="13"/>
-      <c r="P482" s="13"/>
+      <c r="P482" s="38"/>
       <c r="Q482" s="13"/>
       <c r="R482" s="14"/>
       <c r="S482" s="38"/>
@@ -23351,7 +23375,7 @@
       <c r="M483" s="13"/>
       <c r="N483" s="13"/>
       <c r="O483" s="13"/>
-      <c r="P483" s="13"/>
+      <c r="P483" s="38"/>
       <c r="Q483" s="13"/>
       <c r="R483" s="14"/>
       <c r="S483" s="38"/>
@@ -23368,7 +23392,7 @@
       <c r="M484" s="13"/>
       <c r="N484" s="13"/>
       <c r="O484" s="13"/>
-      <c r="P484" s="13"/>
+      <c r="P484" s="38"/>
       <c r="Q484" s="13"/>
       <c r="R484" s="14"/>
       <c r="S484" s="38"/>
@@ -23385,7 +23409,7 @@
       <c r="M485" s="13"/>
       <c r="N485" s="13"/>
       <c r="O485" s="13"/>
-      <c r="P485" s="13"/>
+      <c r="P485" s="38"/>
       <c r="Q485" s="13"/>
       <c r="R485" s="14"/>
       <c r="S485" s="38"/>
@@ -23402,7 +23426,7 @@
       <c r="M486" s="13"/>
       <c r="N486" s="13"/>
       <c r="O486" s="13"/>
-      <c r="P486" s="13"/>
+      <c r="P486" s="38"/>
       <c r="Q486" s="13"/>
       <c r="R486" s="14"/>
       <c r="S486" s="38"/>
@@ -23419,7 +23443,7 @@
       <c r="M487" s="13"/>
       <c r="N487" s="13"/>
       <c r="O487" s="13"/>
-      <c r="P487" s="13"/>
+      <c r="P487" s="38"/>
       <c r="Q487" s="13"/>
       <c r="R487" s="14"/>
       <c r="S487" s="38"/>
@@ -23436,7 +23460,7 @@
       <c r="M488" s="13"/>
       <c r="N488" s="13"/>
       <c r="O488" s="13"/>
-      <c r="P488" s="13"/>
+      <c r="P488" s="38"/>
       <c r="Q488" s="13"/>
       <c r="R488" s="14"/>
       <c r="S488" s="38"/>
@@ -23453,7 +23477,7 @@
       <c r="M489" s="13"/>
       <c r="N489" s="13"/>
       <c r="O489" s="13"/>
-      <c r="P489" s="13"/>
+      <c r="P489" s="38"/>
       <c r="Q489" s="13"/>
       <c r="R489" s="14"/>
       <c r="S489" s="38"/>
@@ -23470,7 +23494,7 @@
       <c r="M490" s="13"/>
       <c r="N490" s="13"/>
       <c r="O490" s="13"/>
-      <c r="P490" s="13"/>
+      <c r="P490" s="38"/>
       <c r="Q490" s="13"/>
       <c r="R490" s="14"/>
       <c r="S490" s="38"/>
@@ -23487,7 +23511,7 @@
       <c r="M491" s="13"/>
       <c r="N491" s="13"/>
       <c r="O491" s="13"/>
-      <c r="P491" s="13"/>
+      <c r="P491" s="38"/>
       <c r="Q491" s="13"/>
       <c r="R491" s="14"/>
       <c r="S491" s="38"/>
@@ -23504,7 +23528,7 @@
       <c r="M492" s="13"/>
       <c r="N492" s="13"/>
       <c r="O492" s="13"/>
-      <c r="P492" s="13"/>
+      <c r="P492" s="38"/>
       <c r="Q492" s="13"/>
       <c r="R492" s="14"/>
       <c r="S492" s="38"/>
@@ -23521,7 +23545,7 @@
       <c r="M493" s="13"/>
       <c r="N493" s="13"/>
       <c r="O493" s="13"/>
-      <c r="P493" s="13"/>
+      <c r="P493" s="38"/>
       <c r="Q493" s="13"/>
       <c r="R493" s="14"/>
       <c r="S493" s="38"/>
@@ -23538,7 +23562,7 @@
       <c r="M494" s="13"/>
       <c r="N494" s="13"/>
       <c r="O494" s="13"/>
-      <c r="P494" s="13"/>
+      <c r="P494" s="38"/>
       <c r="Q494" s="13"/>
       <c r="R494" s="14"/>
       <c r="S494" s="38"/>
@@ -23555,7 +23579,7 @@
       <c r="M495" s="13"/>
       <c r="N495" s="13"/>
       <c r="O495" s="13"/>
-      <c r="P495" s="13"/>
+      <c r="P495" s="38"/>
       <c r="Q495" s="13"/>
       <c r="R495" s="14"/>
       <c r="S495" s="38"/>
@@ -23572,7 +23596,7 @@
       <c r="M496" s="13"/>
       <c r="N496" s="13"/>
       <c r="O496" s="13"/>
-      <c r="P496" s="13"/>
+      <c r="P496" s="38"/>
       <c r="Q496" s="13"/>
       <c r="R496" s="14"/>
       <c r="S496" s="38"/>
@@ -23589,7 +23613,7 @@
       <c r="M497" s="13"/>
       <c r="N497" s="13"/>
       <c r="O497" s="13"/>
-      <c r="P497" s="13"/>
+      <c r="P497" s="38"/>
       <c r="Q497" s="13"/>
       <c r="R497" s="14"/>
       <c r="S497" s="38"/>
@@ -23606,7 +23630,7 @@
       <c r="M498" s="13"/>
       <c r="N498" s="13"/>
       <c r="O498" s="13"/>
-      <c r="P498" s="13"/>
+      <c r="P498" s="38"/>
       <c r="Q498" s="13"/>
       <c r="R498" s="14"/>
       <c r="S498" s="38"/>
@@ -23623,7 +23647,7 @@
       <c r="M499" s="13"/>
       <c r="N499" s="13"/>
       <c r="O499" s="13"/>
-      <c r="P499" s="13"/>
+      <c r="P499" s="38"/>
       <c r="Q499" s="13"/>
       <c r="R499" s="14"/>
       <c r="S499" s="38"/>
@@ -23640,7 +23664,7 @@
       <c r="M500" s="13"/>
       <c r="N500" s="13"/>
       <c r="O500" s="13"/>
-      <c r="P500" s="13"/>
+      <c r="P500" s="38"/>
       <c r="Q500" s="13"/>
       <c r="R500" s="14"/>
       <c r="S500" s="38"/>
@@ -23657,7 +23681,7 @@
       <c r="M501" s="13"/>
       <c r="N501" s="13"/>
       <c r="O501" s="13"/>
-      <c r="P501" s="13"/>
+      <c r="P501" s="38"/>
       <c r="Q501" s="13"/>
       <c r="R501" s="14"/>
       <c r="S501" s="38"/>
@@ -23674,7 +23698,7 @@
       <c r="M502" s="13"/>
       <c r="N502" s="13"/>
       <c r="O502" s="13"/>
-      <c r="P502" s="13"/>
+      <c r="P502" s="38"/>
       <c r="Q502" s="13"/>
       <c r="R502" s="14"/>
       <c r="S502" s="38"/>
@@ -23691,7 +23715,7 @@
       <c r="M503" s="13"/>
       <c r="N503" s="13"/>
       <c r="O503" s="13"/>
-      <c r="P503" s="13"/>
+      <c r="P503" s="38"/>
       <c r="Q503" s="13"/>
       <c r="R503" s="14"/>
       <c r="S503" s="38"/>
@@ -23708,7 +23732,7 @@
       <c r="M504" s="13"/>
       <c r="N504" s="13"/>
       <c r="O504" s="13"/>
-      <c r="P504" s="13"/>
+      <c r="P504" s="38"/>
       <c r="Q504" s="13"/>
       <c r="R504" s="14"/>
       <c r="S504" s="38"/>
@@ -23725,7 +23749,7 @@
       <c r="M505" s="13"/>
       <c r="N505" s="13"/>
       <c r="O505" s="13"/>
-      <c r="P505" s="13"/>
+      <c r="P505" s="38"/>
       <c r="Q505" s="13"/>
       <c r="R505" s="14"/>
       <c r="S505" s="38"/>
@@ -23742,7 +23766,7 @@
       <c r="M506" s="13"/>
       <c r="N506" s="13"/>
       <c r="O506" s="13"/>
-      <c r="P506" s="13"/>
+      <c r="P506" s="38"/>
       <c r="Q506" s="13"/>
       <c r="R506" s="14"/>
       <c r="S506" s="38"/>
@@ -23759,7 +23783,7 @@
       <c r="M507" s="13"/>
       <c r="N507" s="13"/>
       <c r="O507" s="13"/>
-      <c r="P507" s="13"/>
+      <c r="P507" s="38"/>
       <c r="Q507" s="13"/>
       <c r="R507" s="14"/>
       <c r="S507" s="38"/>
@@ -23776,7 +23800,7 @@
       <c r="M508" s="13"/>
       <c r="N508" s="13"/>
       <c r="O508" s="13"/>
-      <c r="P508" s="13"/>
+      <c r="P508" s="38"/>
       <c r="Q508" s="13"/>
       <c r="R508" s="14"/>
       <c r="S508" s="38"/>
@@ -23793,7 +23817,7 @@
       <c r="M509" s="13"/>
       <c r="N509" s="13"/>
       <c r="O509" s="13"/>
-      <c r="P509" s="13"/>
+      <c r="P509" s="38"/>
       <c r="Q509" s="13"/>
       <c r="R509" s="14"/>
       <c r="S509" s="38"/>
@@ -23810,7 +23834,7 @@
       <c r="M510" s="13"/>
       <c r="N510" s="13"/>
       <c r="O510" s="13"/>
-      <c r="P510" s="13"/>
+      <c r="P510" s="38"/>
       <c r="Q510" s="13"/>
       <c r="R510" s="14"/>
       <c r="S510" s="38"/>
@@ -23827,7 +23851,7 @@
       <c r="M511" s="13"/>
       <c r="N511" s="13"/>
       <c r="O511" s="13"/>
-      <c r="P511" s="13"/>
+      <c r="P511" s="38"/>
       <c r="Q511" s="13"/>
       <c r="R511" s="14"/>
       <c r="S511" s="38"/>
@@ -23844,7 +23868,7 @@
       <c r="M512" s="13"/>
       <c r="N512" s="13"/>
       <c r="O512" s="13"/>
-      <c r="P512" s="13"/>
+      <c r="P512" s="38"/>
       <c r="Q512" s="13"/>
       <c r="R512" s="14"/>
       <c r="S512" s="38"/>
@@ -23861,7 +23885,7 @@
       <c r="M513" s="13"/>
       <c r="N513" s="13"/>
       <c r="O513" s="13"/>
-      <c r="P513" s="13"/>
+      <c r="P513" s="38"/>
       <c r="Q513" s="13"/>
       <c r="R513" s="14"/>
       <c r="S513" s="38"/>
@@ -23878,7 +23902,7 @@
       <c r="M514" s="13"/>
       <c r="N514" s="13"/>
       <c r="O514" s="13"/>
-      <c r="P514" s="13"/>
+      <c r="P514" s="38"/>
       <c r="Q514" s="13"/>
       <c r="R514" s="14"/>
       <c r="S514" s="38"/>
@@ -23895,7 +23919,7 @@
       <c r="M515" s="13"/>
       <c r="N515" s="13"/>
       <c r="O515" s="13"/>
-      <c r="P515" s="13"/>
+      <c r="P515" s="38"/>
       <c r="Q515" s="13"/>
       <c r="R515" s="14"/>
       <c r="S515" s="38"/>
@@ -23912,7 +23936,7 @@
       <c r="M516" s="13"/>
       <c r="N516" s="13"/>
       <c r="O516" s="13"/>
-      <c r="P516" s="13"/>
+      <c r="P516" s="38"/>
       <c r="Q516" s="13"/>
       <c r="R516" s="14"/>
       <c r="S516" s="38"/>
@@ -23929,7 +23953,7 @@
       <c r="M517" s="13"/>
       <c r="N517" s="13"/>
       <c r="O517" s="13"/>
-      <c r="P517" s="13"/>
+      <c r="P517" s="38"/>
       <c r="Q517" s="13"/>
       <c r="R517" s="14"/>
       <c r="S517" s="38"/>
@@ -23946,7 +23970,7 @@
       <c r="M518" s="13"/>
       <c r="N518" s="13"/>
       <c r="O518" s="13"/>
-      <c r="P518" s="13"/>
+      <c r="P518" s="38"/>
       <c r="Q518" s="13"/>
       <c r="R518" s="14"/>
       <c r="S518" s="38"/>
@@ -23963,7 +23987,7 @@
       <c r="M519" s="13"/>
       <c r="N519" s="13"/>
       <c r="O519" s="13"/>
-      <c r="P519" s="13"/>
+      <c r="P519" s="38"/>
       <c r="Q519" s="13"/>
       <c r="R519" s="14"/>
       <c r="S519" s="38"/>
@@ -23980,7 +24004,7 @@
       <c r="M520" s="13"/>
       <c r="N520" s="13"/>
       <c r="O520" s="13"/>
-      <c r="P520" s="13"/>
+      <c r="P520" s="38"/>
       <c r="Q520" s="13"/>
       <c r="R520" s="14"/>
       <c r="S520" s="38"/>
@@ -23997,7 +24021,7 @@
       <c r="M521" s="13"/>
       <c r="N521" s="13"/>
       <c r="O521" s="13"/>
-      <c r="P521" s="13"/>
+      <c r="P521" s="38"/>
       <c r="Q521" s="13"/>
       <c r="R521" s="14"/>
       <c r="S521" s="38"/>
@@ -24014,7 +24038,7 @@
       <c r="M522" s="13"/>
       <c r="N522" s="13"/>
       <c r="O522" s="13"/>
-      <c r="P522" s="13"/>
+      <c r="P522" s="38"/>
       <c r="Q522" s="13"/>
       <c r="R522" s="14"/>
       <c r="S522" s="38"/>
@@ -24031,7 +24055,7 @@
       <c r="M523" s="13"/>
       <c r="N523" s="13"/>
       <c r="O523" s="13"/>
-      <c r="P523" s="13"/>
+      <c r="P523" s="38"/>
       <c r="Q523" s="13"/>
       <c r="R523" s="14"/>
       <c r="S523" s="38"/>
@@ -24048,7 +24072,7 @@
       <c r="M524" s="13"/>
       <c r="N524" s="13"/>
       <c r="O524" s="13"/>
-      <c r="P524" s="13"/>
+      <c r="P524" s="38"/>
       <c r="Q524" s="13"/>
       <c r="R524" s="14"/>
       <c r="S524" s="38"/>
@@ -24065,7 +24089,7 @@
       <c r="M525" s="13"/>
       <c r="N525" s="13"/>
       <c r="O525" s="13"/>
-      <c r="P525" s="13"/>
+      <c r="P525" s="38"/>
       <c r="Q525" s="13"/>
       <c r="R525" s="14"/>
       <c r="S525" s="38"/>
@@ -24082,7 +24106,7 @@
       <c r="M526" s="13"/>
       <c r="N526" s="13"/>
       <c r="O526" s="13"/>
-      <c r="P526" s="13"/>
+      <c r="P526" s="38"/>
       <c r="Q526" s="13"/>
       <c r="R526" s="14"/>
       <c r="S526" s="38"/>
@@ -24099,7 +24123,7 @@
       <c r="M527" s="13"/>
       <c r="N527" s="13"/>
       <c r="O527" s="13"/>
-      <c r="P527" s="13"/>
+      <c r="P527" s="38"/>
       <c r="Q527" s="13"/>
       <c r="R527" s="14"/>
       <c r="S527" s="38"/>
@@ -24116,7 +24140,7 @@
       <c r="M528" s="13"/>
       <c r="N528" s="13"/>
       <c r="O528" s="13"/>
-      <c r="P528" s="13"/>
+      <c r="P528" s="38"/>
       <c r="Q528" s="13"/>
       <c r="R528" s="14"/>
       <c r="S528" s="38"/>
@@ -24133,7 +24157,7 @@
       <c r="M529" s="13"/>
       <c r="N529" s="13"/>
       <c r="O529" s="13"/>
-      <c r="P529" s="13"/>
+      <c r="P529" s="38"/>
       <c r="Q529" s="13"/>
       <c r="R529" s="14"/>
       <c r="S529" s="38"/>
@@ -24150,7 +24174,7 @@
       <c r="M530" s="13"/>
       <c r="N530" s="13"/>
       <c r="O530" s="13"/>
-      <c r="P530" s="13"/>
+      <c r="P530" s="38"/>
       <c r="Q530" s="13"/>
       <c r="R530" s="14"/>
       <c r="S530" s="38"/>
@@ -24167,7 +24191,7 @@
       <c r="M531" s="13"/>
       <c r="N531" s="13"/>
       <c r="O531" s="13"/>
-      <c r="P531" s="13"/>
+      <c r="P531" s="38"/>
       <c r="Q531" s="13"/>
       <c r="R531" s="14"/>
       <c r="S531" s="38"/>
@@ -24184,7 +24208,7 @@
       <c r="M532" s="13"/>
       <c r="N532" s="13"/>
       <c r="O532" s="13"/>
-      <c r="P532" s="13"/>
+      <c r="P532" s="38"/>
       <c r="Q532" s="13"/>
       <c r="R532" s="14"/>
       <c r="S532" s="38"/>
@@ -24201,7 +24225,7 @@
       <c r="M533" s="13"/>
       <c r="N533" s="13"/>
       <c r="O533" s="13"/>
-      <c r="P533" s="13"/>
+      <c r="P533" s="38"/>
       <c r="Q533" s="13"/>
       <c r="R533" s="14"/>
       <c r="S533" s="38"/>
@@ -24218,7 +24242,7 @@
       <c r="M534" s="13"/>
       <c r="N534" s="13"/>
       <c r="O534" s="13"/>
-      <c r="P534" s="13"/>
+      <c r="P534" s="38"/>
       <c r="Q534" s="13"/>
       <c r="R534" s="14"/>
       <c r="S534" s="38"/>
@@ -24235,7 +24259,7 @@
       <c r="M535" s="13"/>
       <c r="N535" s="13"/>
       <c r="O535" s="13"/>
-      <c r="P535" s="13"/>
+      <c r="P535" s="38"/>
       <c r="Q535" s="13"/>
       <c r="R535" s="14"/>
       <c r="S535" s="38"/>
@@ -24252,7 +24276,7 @@
       <c r="M536" s="13"/>
       <c r="N536" s="13"/>
       <c r="O536" s="13"/>
-      <c r="P536" s="13"/>
+      <c r="P536" s="38"/>
       <c r="Q536" s="13"/>
       <c r="R536" s="14"/>
       <c r="S536" s="38"/>
@@ -24269,7 +24293,7 @@
       <c r="M537" s="13"/>
       <c r="N537" s="13"/>
       <c r="O537" s="13"/>
-      <c r="P537" s="13"/>
+      <c r="P537" s="38"/>
       <c r="Q537" s="13"/>
       <c r="R537" s="14"/>
       <c r="S537" s="38"/>
@@ -24286,7 +24310,7 @@
       <c r="M538" s="13"/>
       <c r="N538" s="13"/>
       <c r="O538" s="13"/>
-      <c r="P538" s="13"/>
+      <c r="P538" s="38"/>
       <c r="Q538" s="13"/>
       <c r="R538" s="14"/>
       <c r="S538" s="38"/>
@@ -24303,7 +24327,7 @@
       <c r="M539" s="13"/>
       <c r="N539" s="13"/>
       <c r="O539" s="13"/>
-      <c r="P539" s="13"/>
+      <c r="P539" s="38"/>
       <c r="Q539" s="13"/>
       <c r="R539" s="14"/>
       <c r="S539" s="38"/>
@@ -24320,7 +24344,7 @@
       <c r="M540" s="13"/>
       <c r="N540" s="13"/>
       <c r="O540" s="13"/>
-      <c r="P540" s="13"/>
+      <c r="P540" s="38"/>
       <c r="Q540" s="13"/>
       <c r="R540" s="14"/>
       <c r="S540" s="38"/>
@@ -24337,7 +24361,7 @@
       <c r="M541" s="13"/>
       <c r="N541" s="13"/>
       <c r="O541" s="13"/>
-      <c r="P541" s="13"/>
+      <c r="P541" s="38"/>
       <c r="Q541" s="13"/>
       <c r="R541" s="14"/>
       <c r="S541" s="38"/>
@@ -24354,7 +24378,7 @@
       <c r="M542" s="13"/>
       <c r="N542" s="13"/>
       <c r="O542" s="13"/>
-      <c r="P542" s="13"/>
+      <c r="P542" s="38"/>
       <c r="Q542" s="13"/>
       <c r="R542" s="14"/>
       <c r="S542" s="38"/>
@@ -24371,7 +24395,7 @@
       <c r="M543" s="13"/>
       <c r="N543" s="13"/>
       <c r="O543" s="13"/>
-      <c r="P543" s="13"/>
+      <c r="P543" s="38"/>
       <c r="Q543" s="13"/>
       <c r="R543" s="14"/>
       <c r="S543" s="38"/>
@@ -24388,7 +24412,7 @@
       <c r="M544" s="13"/>
       <c r="N544" s="13"/>
       <c r="O544" s="13"/>
-      <c r="P544" s="13"/>
+      <c r="P544" s="38"/>
       <c r="Q544" s="13"/>
       <c r="R544" s="14"/>
       <c r="S544" s="38"/>
@@ -24405,7 +24429,7 @@
       <c r="M545" s="13"/>
       <c r="N545" s="13"/>
       <c r="O545" s="13"/>
-      <c r="P545" s="13"/>
+      <c r="P545" s="38"/>
       <c r="Q545" s="13"/>
       <c r="R545" s="14"/>
       <c r="S545" s="38"/>
@@ -24422,7 +24446,7 @@
       <c r="M546" s="13"/>
       <c r="N546" s="13"/>
       <c r="O546" s="13"/>
-      <c r="P546" s="13"/>
+      <c r="P546" s="38"/>
       <c r="Q546" s="13"/>
       <c r="R546" s="14"/>
       <c r="S546" s="38"/>
@@ -24439,7 +24463,7 @@
       <c r="M547" s="13"/>
       <c r="N547" s="13"/>
       <c r="O547" s="13"/>
-      <c r="P547" s="13"/>
+      <c r="P547" s="38"/>
       <c r="Q547" s="13"/>
       <c r="R547" s="14"/>
       <c r="S547" s="38"/>
@@ -24456,7 +24480,7 @@
       <c r="M548" s="13"/>
       <c r="N548" s="13"/>
       <c r="O548" s="13"/>
-      <c r="P548" s="13"/>
+      <c r="P548" s="38"/>
       <c r="Q548" s="13"/>
       <c r="R548" s="14"/>
       <c r="S548" s="38"/>
@@ -24473,7 +24497,7 @@
       <c r="M549" s="13"/>
       <c r="N549" s="13"/>
       <c r="O549" s="13"/>
-      <c r="P549" s="13"/>
+      <c r="P549" s="38"/>
       <c r="Q549" s="13"/>
       <c r="R549" s="14"/>
       <c r="S549" s="38"/>
@@ -24490,7 +24514,7 @@
       <c r="M550" s="13"/>
       <c r="N550" s="13"/>
       <c r="O550" s="13"/>
-      <c r="P550" s="13"/>
+      <c r="P550" s="38"/>
       <c r="Q550" s="13"/>
       <c r="R550" s="14"/>
       <c r="S550" s="38"/>
@@ -24507,7 +24531,7 @@
       <c r="M551" s="13"/>
       <c r="N551" s="13"/>
       <c r="O551" s="13"/>
-      <c r="P551" s="13"/>
+      <c r="P551" s="38"/>
       <c r="Q551" s="13"/>
       <c r="R551" s="14"/>
       <c r="S551" s="38"/>
@@ -24524,7 +24548,7 @@
       <c r="M552" s="13"/>
       <c r="N552" s="13"/>
       <c r="O552" s="13"/>
-      <c r="P552" s="13"/>
+      <c r="P552" s="38"/>
       <c r="Q552" s="13"/>
       <c r="R552" s="14"/>
       <c r="S552" s="38"/>
@@ -24541,7 +24565,7 @@
       <c r="M553" s="13"/>
       <c r="N553" s="13"/>
       <c r="O553" s="13"/>
-      <c r="P553" s="13"/>
+      <c r="P553" s="38"/>
       <c r="Q553" s="13"/>
       <c r="R553" s="14"/>
       <c r="S553" s="38"/>
@@ -24558,7 +24582,7 @@
       <c r="M554" s="13"/>
       <c r="N554" s="13"/>
       <c r="O554" s="13"/>
-      <c r="P554" s="13"/>
+      <c r="P554" s="38"/>
       <c r="Q554" s="13"/>
       <c r="R554" s="14"/>
       <c r="S554" s="38"/>
@@ -24575,7 +24599,7 @@
       <c r="M555" s="13"/>
       <c r="N555" s="13"/>
       <c r="O555" s="13"/>
-      <c r="P555" s="13"/>
+      <c r="P555" s="38"/>
       <c r="Q555" s="13"/>
       <c r="R555" s="14"/>
       <c r="S555" s="38"/>
@@ -24592,7 +24616,7 @@
       <c r="M556" s="13"/>
       <c r="N556" s="13"/>
       <c r="O556" s="13"/>
-      <c r="P556" s="13"/>
+      <c r="P556" s="38"/>
       <c r="Q556" s="13"/>
       <c r="R556" s="14"/>
       <c r="S556" s="38"/>
@@ -24609,7 +24633,7 @@
       <c r="M557" s="13"/>
       <c r="N557" s="13"/>
       <c r="O557" s="13"/>
-      <c r="P557" s="13"/>
+      <c r="P557" s="38"/>
       <c r="Q557" s="13"/>
       <c r="R557" s="14"/>
       <c r="S557" s="38"/>
@@ -24626,7 +24650,7 @@
       <c r="M558" s="13"/>
       <c r="N558" s="13"/>
       <c r="O558" s="13"/>
-      <c r="P558" s="13"/>
+      <c r="P558" s="38"/>
       <c r="Q558" s="13"/>
       <c r="R558" s="14"/>
       <c r="S558" s="38"/>
@@ -24643,7 +24667,7 @@
       <c r="M559" s="13"/>
       <c r="N559" s="13"/>
       <c r="O559" s="13"/>
-      <c r="P559" s="13"/>
+      <c r="P559" s="38"/>
       <c r="Q559" s="13"/>
       <c r="R559" s="14"/>
       <c r="S559" s="38"/>
@@ -24660,7 +24684,7 @@
       <c r="M560" s="13"/>
       <c r="N560" s="13"/>
       <c r="O560" s="13"/>
-      <c r="P560" s="13"/>
+      <c r="P560" s="38"/>
       <c r="Q560" s="13"/>
       <c r="R560" s="14"/>
       <c r="S560" s="38"/>
@@ -24677,7 +24701,7 @@
       <c r="M561" s="13"/>
       <c r="N561" s="13"/>
       <c r="O561" s="13"/>
-      <c r="P561" s="13"/>
+      <c r="P561" s="38"/>
       <c r="Q561" s="13"/>
       <c r="R561" s="14"/>
       <c r="S561" s="38"/>
@@ -24694,7 +24718,7 @@
       <c r="M562" s="13"/>
       <c r="N562" s="13"/>
       <c r="O562" s="13"/>
-      <c r="P562" s="13"/>
+      <c r="P562" s="38"/>
       <c r="Q562" s="13"/>
       <c r="R562" s="14"/>
       <c r="S562" s="38"/>
@@ -24711,7 +24735,7 @@
       <c r="M563" s="13"/>
       <c r="N563" s="13"/>
       <c r="O563" s="13"/>
-      <c r="P563" s="13"/>
+      <c r="P563" s="38"/>
       <c r="Q563" s="13"/>
       <c r="R563" s="14"/>
       <c r="S563" s="38"/>
@@ -24728,7 +24752,7 @@
       <c r="M564" s="13"/>
       <c r="N564" s="13"/>
       <c r="O564" s="13"/>
-      <c r="P564" s="13"/>
+      <c r="P564" s="38"/>
       <c r="Q564" s="13"/>
       <c r="R564" s="14"/>
       <c r="S564" s="38"/>
@@ -24745,7 +24769,7 @@
       <c r="M565" s="13"/>
       <c r="N565" s="13"/>
       <c r="O565" s="13"/>
-      <c r="P565" s="13"/>
+      <c r="P565" s="38"/>
       <c r="Q565" s="13"/>
       <c r="R565" s="14"/>
       <c r="S565" s="38"/>
@@ -24762,7 +24786,7 @@
       <c r="M566" s="13"/>
       <c r="N566" s="13"/>
       <c r="O566" s="13"/>
-      <c r="P566" s="13"/>
+      <c r="P566" s="38"/>
       <c r="Q566" s="13"/>
       <c r="R566" s="14"/>
       <c r="S566" s="38"/>
@@ -24779,7 +24803,7 @@
       <c r="M567" s="13"/>
       <c r="N567" s="13"/>
       <c r="O567" s="13"/>
-      <c r="P567" s="13"/>
+      <c r="P567" s="38"/>
       <c r="Q567" s="13"/>
       <c r="R567" s="14"/>
       <c r="S567" s="38"/>
@@ -24796,7 +24820,7 @@
       <c r="M568" s="13"/>
       <c r="N568" s="13"/>
       <c r="O568" s="13"/>
-      <c r="P568" s="13"/>
+      <c r="P568" s="38"/>
       <c r="Q568" s="13"/>
       <c r="R568" s="14"/>
       <c r="S568" s="38"/>
@@ -24813,7 +24837,7 @@
       <c r="M569" s="13"/>
       <c r="N569" s="13"/>
       <c r="O569" s="13"/>
-      <c r="P569" s="13"/>
+      <c r="P569" s="38"/>
       <c r="Q569" s="13"/>
       <c r="R569" s="14"/>
       <c r="S569" s="38"/>
@@ -24830,7 +24854,7 @@
       <c r="M570" s="13"/>
       <c r="N570" s="13"/>
       <c r="O570" s="13"/>
-      <c r="P570" s="13"/>
+      <c r="P570" s="38"/>
       <c r="Q570" s="13"/>
       <c r="R570" s="14"/>
       <c r="S570" s="38"/>
@@ -24847,7 +24871,7 @@
       <c r="M571" s="13"/>
       <c r="N571" s="13"/>
       <c r="O571" s="13"/>
-      <c r="P571" s="13"/>
+      <c r="P571" s="38"/>
       <c r="Q571" s="13"/>
       <c r="R571" s="14"/>
       <c r="S571" s="38"/>
@@ -24864,7 +24888,7 @@
       <c r="M572" s="13"/>
       <c r="N572" s="13"/>
       <c r="O572" s="13"/>
-      <c r="P572" s="13"/>
+      <c r="P572" s="38"/>
       <c r="Q572" s="13"/>
       <c r="R572" s="14"/>
       <c r="S572" s="38"/>
@@ -24881,7 +24905,7 @@
       <c r="M573" s="13"/>
       <c r="N573" s="13"/>
       <c r="O573" s="13"/>
-      <c r="P573" s="13"/>
+      <c r="P573" s="38"/>
       <c r="Q573" s="13"/>
       <c r="R573" s="14"/>
       <c r="S573" s="38"/>
@@ -24898,7 +24922,7 @@
       <c r="M574" s="13"/>
       <c r="N574" s="13"/>
       <c r="O574" s="13"/>
-      <c r="P574" s="13"/>
+      <c r="P574" s="38"/>
       <c r="Q574" s="13"/>
       <c r="R574" s="14"/>
       <c r="S574" s="38"/>
@@ -24915,7 +24939,7 @@
       <c r="M575" s="13"/>
       <c r="N575" s="13"/>
       <c r="O575" s="13"/>
-      <c r="P575" s="13"/>
+      <c r="P575" s="38"/>
       <c r="Q575" s="13"/>
       <c r="R575" s="14"/>
       <c r="S575" s="38"/>
@@ -24932,7 +24956,7 @@
       <c r="M576" s="13"/>
       <c r="N576" s="13"/>
       <c r="O576" s="13"/>
-      <c r="P576" s="13"/>
+      <c r="P576" s="38"/>
       <c r="Q576" s="13"/>
       <c r="R576" s="14"/>
       <c r="S576" s="38"/>
@@ -24949,7 +24973,7 @@
       <c r="M577" s="13"/>
       <c r="N577" s="13"/>
       <c r="O577" s="13"/>
-      <c r="P577" s="13"/>
+      <c r="P577" s="38"/>
       <c r="Q577" s="13"/>
       <c r="R577" s="14"/>
       <c r="S577" s="38"/>
@@ -24966,7 +24990,7 @@
       <c r="M578" s="13"/>
       <c r="N578" s="13"/>
       <c r="O578" s="13"/>
-      <c r="P578" s="13"/>
+      <c r="P578" s="38"/>
       <c r="Q578" s="13"/>
       <c r="R578" s="14"/>
       <c r="S578" s="38"/>
@@ -24983,7 +25007,7 @@
       <c r="M579" s="13"/>
       <c r="N579" s="13"/>
       <c r="O579" s="13"/>
-      <c r="P579" s="13"/>
+      <c r="P579" s="38"/>
       <c r="Q579" s="13"/>
       <c r="R579" s="14"/>
       <c r="S579" s="38"/>
@@ -25000,7 +25024,7 @@
       <c r="M580" s="13"/>
       <c r="N580" s="13"/>
       <c r="O580" s="13"/>
-      <c r="P580" s="13"/>
+      <c r="P580" s="38"/>
       <c r="Q580" s="13"/>
       <c r="R580" s="14"/>
       <c r="S580" s="38"/>
@@ -25017,7 +25041,7 @@
       <c r="M581" s="13"/>
       <c r="N581" s="13"/>
       <c r="O581" s="13"/>
-      <c r="P581" s="13"/>
+      <c r="P581" s="38"/>
       <c r="Q581" s="13"/>
       <c r="R581" s="14"/>
       <c r="S581" s="38"/>
@@ -25034,7 +25058,7 @@
       <c r="M582" s="13"/>
       <c r="N582" s="13"/>
       <c r="O582" s="13"/>
-      <c r="P582" s="13"/>
+      <c r="P582" s="38"/>
       <c r="Q582" s="13"/>
       <c r="R582" s="14"/>
       <c r="S582" s="38"/>
@@ -25051,7 +25075,7 @@
       <c r="M583" s="13"/>
       <c r="N583" s="13"/>
       <c r="O583" s="13"/>
-      <c r="P583" s="13"/>
+      <c r="P583" s="38"/>
       <c r="Q583" s="13"/>
       <c r="R583" s="14"/>
       <c r="S583" s="38"/>

</xml_diff>